<commit_message>
get product count method updated
</commit_message>
<xml_diff>
--- a/Documents/Template/9/Requirement/test.xlsx
+++ b/Documents/Template/9/Requirement/test.xlsx
@@ -332,27 +332,29 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="27" min="18" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -445,7 +447,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
voided product group by customer sku
</commit_message>
<xml_diff>
--- a/Documents/Template/9/Requirement/test.xlsx
+++ b/Documents/Template/9/Requirement/test.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">TROUBLESHOOT/REPAIR-MRI CONTROLS</t>
   </si>
   <si>
-    <t xml:space="preserve">MRI</t>
+    <t xml:space="preserve">iphone123</t>
   </si>
   <si>
     <t xml:space="preserve">Unknown (DO NOT USE)</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">TROUBLESHOOT-RTU 11A CONTROLLERS OFFLINE</t>
   </si>
   <si>
-    <t xml:space="preserve">INVOICE 5227</t>
+    <t xml:space="preserve">iphone456</t>
   </si>
   <si>
     <t xml:space="preserve">1209183</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">INK AND PAPER FOR NEW PRINTERS</t>
   </si>
   <si>
-    <t xml:space="preserve">0240-080-231</t>
+    <t xml:space="preserve">iphone789</t>
   </si>
   <si>
     <t xml:space="preserve">STRYKER ENDO</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">GARRETT VASCULAR DILATOR SET/9 8 1/2"</t>
   </si>
   <si>
-    <t xml:space="preserve">MB256</t>
+    <t xml:space="preserve">MRI21</t>
   </si>
   <si>
     <t xml:space="preserve">AESCULAP INC</t>
@@ -285,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +300,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -332,7 +336,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,23 +443,23 @@
       <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="4" t="n">
-        <v>9</v>
+      <c r="J2" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="6" t="n">
         <v>3000</v>
       </c>
-      <c r="M2" s="5" t="n">
+      <c r="M2" s="6" t="n">
         <v>3000</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -498,23 +502,23 @@
       <c r="F3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="4" t="n">
-        <v>10</v>
+      <c r="J3" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="6" t="n">
         <v>474.5</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="6" t="n">
         <v>474.5</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -557,7 +561,7 @@
       <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -566,16 +570,16 @@
       <c r="I4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="4" t="n">
-        <v>10</v>
+      <c r="J4" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <v>241</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="6" t="n">
         <v>482</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -618,7 +622,7 @@
       <c r="F5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -627,16 +631,16 @@
       <c r="I5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="5" t="n">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <v>171.79</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="6" t="n">
         <v>171.79</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -688,16 +692,16 @@
       <c r="I6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="6" t="n">
         <v>215</v>
       </c>
       <c r="N6" s="2" t="s">

</xml_diff>

<commit_message>
changes in pr engine
</commit_message>
<xml_diff>
--- a/Documents/Template/9/Requirement/test.xlsx
+++ b/Documents/Template/9/Requirement/test.xlsx
@@ -336,29 +336,29 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="64.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.7142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.765306122449"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="27" min="18" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -451,7 +451,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>24</v>

</xml_diff>